<commit_message>
updated with Mysql dependency in pom and mysqltest
</commit_message>
<xml_diff>
--- a/src/test/resources/Test.xlsx
+++ b/src/test/resources/Test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium With Java\GitStuff\imf.webautomation.com\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\My-created-framework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE165FFA-6967-4669-AD50-2C6E78449B40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177264ED-FADD-4DC3-B8BC-F2A67B1F4460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>TestData8</t>
   </si>
   <si>
-    <t>imfpagetitletest</t>
-  </si>
-  <si>
     <t>International Monetary Fund - Homepage</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>Iran, Islamic Republic of</t>
+  </si>
+  <si>
+    <t>imfpagetitletest_excel</t>
   </si>
 </sst>
 </file>
@@ -400,12 +400,12 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
@@ -467,25 +467,25 @@
     </row>
     <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>

</xml_diff>